<commit_message>
add two img and develop lab
</commit_message>
<xml_diff>
--- a/lab_3(excel_+_git)/laba3_VMO11_shchegolkov.xlsx
+++ b/lab_3(excel_+_git)/laba3_VMO11_shchegolkov.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSTU\DSTU_labs_Shchegolkov_Vladimir\lab_3(excel_+_git)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F63B9E-9EAB-4A64-AFB9-CA227BBE95FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985FAFAE-8648-43DA-890B-6D7470B1BA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{325DE10F-A366-4F5C-B81D-405FC9292D5F}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,21 +158,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -200,53 +193,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -410,34 +356,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,31 +463,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="8">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2</c:v>
@@ -624,34 +570,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -734,22 +680,22 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3</c:v>
@@ -758,7 +704,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,25 +784,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>4</c:v>
@@ -865,7 +811,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1973,10 +1919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A75F90-EA4A-4595-9744-F19FEB9FA521}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2012,27 +1958,27 @@
       </c>
       <c r="B2" s="1">
         <f ca="1">RANDBETWEEN(2,5)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:F11" ca="1" si="0">RANDBETWEEN(2,5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="E2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="F2" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G2" s="3">
         <f ca="1">AVERAGE(B2:F2)</f>
-        <v>2.4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2045,15 +1991,15 @@
       </c>
       <c r="C3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2061,7 +2007,7 @@
       </c>
       <c r="G3" s="3">
         <f t="shared" ref="G3:G11" ca="1" si="2">AVERAGE(B3:F3)</f>
-        <v>2.2000000000000002</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2070,27 +2016,27 @@
       </c>
       <c r="B4" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>2.8</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -2099,15 +2045,15 @@
       </c>
       <c r="B5" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2119,7 +2065,7 @@
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>4.2</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2128,27 +2074,27 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="C6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
       <c r="D6" s="1">
         <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -2157,19 +2103,19 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2177,7 +2123,7 @@
       </c>
       <c r="G7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2186,23 +2132,23 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>2</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" ca="1" si="2"/>
@@ -2215,11 +2161,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2235,7 +2181,7 @@
       </c>
       <c r="G9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2248,11 +2194,11 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>5</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -2264,7 +2210,7 @@
       </c>
       <c r="G10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2273,48 +2219,63 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
       <c r="E11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>3.2</v>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G12" s="4">
+        <f ca="1">MIN(G2:G11)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="4">
+        <f ca="1">MAX(G2:G11)</f>
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <f ca="1">MIN(G2:G11)</f>
+        <v>2.6</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4 D6 E7 B8 B10">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F11">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:G11">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>5</formula>
-    </cfRule>
+  <conditionalFormatting sqref="B2:G11 G12:G13">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2325,13 +2286,16 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>5</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+  <conditionalFormatting sqref="G2:G13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>3</formula>
       <formula>3.999</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>4</formula>
       <formula>4.999</formula>
     </cfRule>

</xml_diff>